<commit_message>
Actualizada la tabla de datos de frijol
</commit_message>
<xml_diff>
--- a/data/frijol.xlsx
+++ b/data/frijol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CETE\Downloads\data\miapa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117EDA45-4D2B-443A-8AEA-F423179CDB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B426C375-4A39-4710-96D8-4106CD85ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,7 +350,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Pendiente el modelo de efectos mixtos
</commit_message>
<xml_diff>
--- a/data/frijol.xlsx
+++ b/data/frijol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CETE\Downloads\data\miapa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B426C375-4A39-4710-96D8-4106CD85ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F42D11B-5615-4896-8932-925FC5E33B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="34">
   <si>
     <t>Jicaro</t>
   </si>
@@ -84,12 +84,51 @@
   <si>
     <t>Bloq</t>
   </si>
+  <si>
+    <t>Loc_Bloq</t>
+  </si>
+  <si>
+    <t>Jicaro_1</t>
+  </si>
+  <si>
+    <t>Jicaro_2</t>
+  </si>
+  <si>
+    <t>Jicaro_3</t>
+  </si>
+  <si>
+    <t>Jicaro_4</t>
+  </si>
+  <si>
+    <t>Rancho_1</t>
+  </si>
+  <si>
+    <t>Rancho_2</t>
+  </si>
+  <si>
+    <t>Rancho_3</t>
+  </si>
+  <si>
+    <t>Rancho_4</t>
+  </si>
+  <si>
+    <t>Estancia_1</t>
+  </si>
+  <si>
+    <t>Estancia_2</t>
+  </si>
+  <si>
+    <t>Estancia_3</t>
+  </si>
+  <si>
+    <t>Estancia_4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +139,11 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -347,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A150" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157:E169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -359,10 +403,11 @@
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="26" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -375,8 +420,11 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -389,8 +437,11 @@
       <c r="D2" s="2">
         <v>405.56</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -403,8 +454,11 @@
       <c r="D3" s="2">
         <v>755.35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -417,8 +471,11 @@
       <c r="D4" s="2">
         <v>348.87</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -431,8 +488,11 @@
       <c r="D5" s="2">
         <v>232.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -445,8 +505,11 @@
       <c r="D6" s="2">
         <v>400.48</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -459,8 +522,11 @@
       <c r="D7" s="2">
         <v>373.49</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -473,8 +539,11 @@
       <c r="D8" s="2">
         <v>265.69</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,8 +556,11 @@
       <c r="D9" s="2">
         <v>529.96</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -501,8 +573,11 @@
       <c r="D10" s="2">
         <v>724.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -515,8 +590,11 @@
       <c r="D11" s="2">
         <v>619.41</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,8 +607,11 @@
       <c r="D12" s="2">
         <v>194.96</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -543,8 +624,11 @@
       <c r="D13" s="2">
         <v>340.16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -557,8 +641,11 @@
       <c r="D14" s="2">
         <v>492.41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -571,8 +658,11 @@
       <c r="D15" s="2">
         <v>375</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -585,8 +675,11 @@
       <c r="D16" s="2">
         <v>526.35</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -599,8 +692,11 @@
       <c r="D17" s="2">
         <v>555.96</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,8 +709,11 @@
       <c r="D18" s="2">
         <v>359.16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,8 +726,11 @@
       <c r="D19" s="2">
         <v>341.65</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -641,8 +743,11 @@
       <c r="D20" s="2">
         <v>526.23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -655,8 +760,11 @@
       <c r="D21" s="2">
         <v>867.97</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -669,8 +777,11 @@
       <c r="D22" s="2">
         <v>266.95999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -683,8 +794,11 @@
       <c r="D23" s="2">
         <v>405.34</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -697,8 +811,11 @@
       <c r="D24" s="2">
         <v>538.13</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -711,8 +828,11 @@
       <c r="D25" s="2">
         <v>687.92</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -725,8 +845,11 @@
       <c r="D26" s="2">
         <v>195.03</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -739,8 +862,11 @@
       <c r="D27" s="2">
         <v>520.01</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -753,8 +879,11 @@
       <c r="D28" s="2">
         <v>442.01</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -767,8 +896,11 @@
       <c r="D29" s="2">
         <v>301.27</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -781,8 +913,11 @@
       <c r="D30" s="2">
         <v>245.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -795,8 +930,11 @@
       <c r="D31" s="2">
         <v>615.70000000000005</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -809,8 +947,11 @@
       <c r="D32" s="2">
         <v>467.32</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -823,8 +964,11 @@
       <c r="D33" s="2">
         <v>209.17</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -837,8 +981,11 @@
       <c r="D34" s="2">
         <v>284.02</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -851,8 +998,11 @@
       <c r="D35" s="2">
         <v>589.54999999999995</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -865,8 +1015,11 @@
       <c r="D36" s="2">
         <v>443.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -879,8 +1032,11 @@
       <c r="D37" s="2">
         <v>345.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -893,8 +1049,11 @@
       <c r="D38" s="2">
         <v>736.51</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -907,8 +1066,11 @@
       <c r="D39" s="2">
         <v>450.99</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -921,8 +1083,11 @@
       <c r="D40" s="2">
         <v>285.66000000000003</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
@@ -935,8 +1100,11 @@
       <c r="D41" s="2">
         <v>600.51</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -949,8 +1117,11 @@
       <c r="D42" s="2">
         <v>481.07</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>0</v>
       </c>
@@ -963,8 +1134,11 @@
       <c r="D43" s="2">
         <v>259.94</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
@@ -977,8 +1151,11 @@
       <c r="D44" s="2">
         <v>458.81</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
@@ -991,8 +1168,11 @@
       <c r="D45" s="2">
         <v>533.27</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
@@ -1005,8 +1185,11 @@
       <c r="D46" s="2">
         <v>465.94</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
@@ -1019,8 +1202,11 @@
       <c r="D47" s="2">
         <v>462.48</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>0</v>
       </c>
@@ -1033,8 +1219,11 @@
       <c r="D48" s="2">
         <v>389.48</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>0</v>
       </c>
@@ -1047,8 +1236,11 @@
       <c r="D49" s="2">
         <v>686.75</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
@@ -1061,8 +1253,11 @@
       <c r="D50" s="2">
         <v>477.13</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +1270,11 @@
       <c r="D51" s="2">
         <v>426.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>0</v>
       </c>
@@ -1089,8 +1287,11 @@
       <c r="D52" s="2">
         <v>452.48</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>0</v>
       </c>
@@ -1103,8 +1304,11 @@
       <c r="D53" s="2">
         <v>492.21</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
@@ -1117,8 +1321,11 @@
       <c r="D54" s="2">
         <v>217.95</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
@@ -1131,8 +1338,11 @@
       <c r="D55" s="2">
         <v>400.02</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
@@ -1145,8 +1355,11 @@
       <c r="D56" s="2">
         <v>284</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -1159,8 +1372,11 @@
       <c r="D57" s="2">
         <v>269.94</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>15</v>
       </c>
@@ -1173,8 +1389,11 @@
       <c r="D58" s="2">
         <v>266.75</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>15</v>
       </c>
@@ -1187,8 +1406,11 @@
       <c r="D59" s="2">
         <v>408.98</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>15</v>
       </c>
@@ -1201,8 +1423,11 @@
       <c r="D60" s="2">
         <v>462.64</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>15</v>
       </c>
@@ -1215,8 +1440,11 @@
       <c r="D61" s="2">
         <v>277.73</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>15</v>
       </c>
@@ -1229,8 +1457,11 @@
       <c r="D62" s="2">
         <v>497.13</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>15</v>
       </c>
@@ -1243,8 +1474,11 @@
       <c r="D63" s="2">
         <v>853.19</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>15</v>
       </c>
@@ -1257,8 +1491,11 @@
       <c r="D64" s="2">
         <v>549.84</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>15</v>
       </c>
@@ -1271,8 +1508,11 @@
       <c r="D65" s="2">
         <v>503.1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>15</v>
       </c>
@@ -1285,8 +1525,11 @@
       <c r="D66" s="2">
         <v>708.12</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>15</v>
       </c>
@@ -1299,8 +1542,11 @@
       <c r="D67" s="2">
         <v>182.53</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>15</v>
       </c>
@@ -1313,8 +1559,11 @@
       <c r="D68" s="2">
         <v>166.55</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>15</v>
       </c>
@@ -1327,8 +1576,11 @@
       <c r="D69" s="2">
         <v>453.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>15</v>
       </c>
@@ -1341,8 +1593,11 @@
       <c r="D70" s="2">
         <v>523.09</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>15</v>
       </c>
@@ -1355,8 +1610,11 @@
       <c r="D71" s="2">
         <v>201.07</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>15</v>
       </c>
@@ -1369,8 +1627,11 @@
       <c r="D72" s="2">
         <v>666.92</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E72" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>15</v>
       </c>
@@ -1383,8 +1644,11 @@
       <c r="D73" s="2">
         <v>276.25</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>15</v>
       </c>
@@ -1397,8 +1661,11 @@
       <c r="D74" s="2">
         <v>265.23</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>15</v>
       </c>
@@ -1411,8 +1678,11 @@
       <c r="D75" s="2">
         <v>383.88</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>15</v>
       </c>
@@ -1425,8 +1695,11 @@
       <c r="D76" s="2">
         <v>325.92</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E76" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>15</v>
       </c>
@@ -1439,8 +1712,11 @@
       <c r="D77" s="2">
         <v>154.22</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E77" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>15</v>
       </c>
@@ -1453,8 +1729,11 @@
       <c r="D78" s="2">
         <v>203.22</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E78" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>15</v>
       </c>
@@ -1467,8 +1746,11 @@
       <c r="D79" s="2">
         <v>338.67</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>15</v>
       </c>
@@ -1481,8 +1763,11 @@
       <c r="D80" s="2">
         <v>797.18</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>15</v>
       </c>
@@ -1495,8 +1780,11 @@
       <c r="D81" s="2">
         <v>425.06</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>15</v>
       </c>
@@ -1509,8 +1797,11 @@
       <c r="D82" s="2">
         <v>151.68</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E82" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>15</v>
       </c>
@@ -1523,8 +1814,11 @@
       <c r="D83" s="2">
         <v>557.82000000000005</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>15</v>
       </c>
@@ -1537,8 +1831,11 @@
       <c r="D84" s="2">
         <v>467.08</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E84" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>15</v>
       </c>
@@ -1551,8 +1848,11 @@
       <c r="D85" s="2">
         <v>361.75</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>15</v>
       </c>
@@ -1565,8 +1865,11 @@
       <c r="D86" s="2">
         <v>300.70999999999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E86" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>15</v>
       </c>
@@ -1579,8 +1882,11 @@
       <c r="D87" s="2">
         <v>287.02999999999997</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>15</v>
       </c>
@@ -1593,8 +1899,11 @@
       <c r="D88" s="2">
         <v>193.46</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>15</v>
       </c>
@@ -1607,8 +1916,11 @@
       <c r="D89" s="2">
         <v>548.41</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>15</v>
       </c>
@@ -1621,8 +1933,11 @@
       <c r="D90" s="2">
         <v>621.4</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>15</v>
       </c>
@@ -1635,8 +1950,11 @@
       <c r="D91" s="2">
         <v>559.49</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E91" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>15</v>
       </c>
@@ -1649,8 +1967,11 @@
       <c r="D92" s="2">
         <v>801.02</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E92" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>15</v>
       </c>
@@ -1663,8 +1984,11 @@
       <c r="D93" s="2">
         <v>147.07</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>15</v>
       </c>
@@ -1677,8 +2001,11 @@
       <c r="D94" s="2">
         <v>213.28</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E94" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>15</v>
       </c>
@@ -1691,8 +2018,11 @@
       <c r="D95" s="2">
         <v>138.54</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>15</v>
       </c>
@@ -1705,8 +2035,11 @@
       <c r="D96" s="2">
         <v>235.65</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E96" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>15</v>
       </c>
@@ -1719,8 +2052,11 @@
       <c r="D97" s="2">
         <v>372.81</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E97" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>15</v>
       </c>
@@ -1733,8 +2069,11 @@
       <c r="D98" s="2">
         <v>461.54</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E98" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>15</v>
       </c>
@@ -1747,8 +2086,11 @@
       <c r="D99" s="2">
         <v>552.94000000000005</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E99" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>15</v>
       </c>
@@ -1761,8 +2103,11 @@
       <c r="D100" s="2">
         <v>312.04000000000002</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>15</v>
       </c>
@@ -1775,8 +2120,11 @@
       <c r="D101" s="2">
         <v>951.19</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E101" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>15</v>
       </c>
@@ -1789,8 +2137,11 @@
       <c r="D102" s="2">
         <v>450.74</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E102" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>15</v>
       </c>
@@ -1803,8 +2154,11 @@
       <c r="D103" s="2">
         <v>320.56</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E103" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>15</v>
       </c>
@@ -1817,8 +2171,11 @@
       <c r="D104" s="2">
         <v>444.88</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>15</v>
       </c>
@@ -1831,8 +2188,11 @@
       <c r="D105" s="2">
         <v>501.63</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E105" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>15</v>
       </c>
@@ -1845,8 +2205,11 @@
       <c r="D106" s="2">
         <v>392</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E106" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>15</v>
       </c>
@@ -1859,8 +2222,11 @@
       <c r="D107" s="2">
         <v>352.18</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E107" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>15</v>
       </c>
@@ -1873,8 +2239,11 @@
       <c r="D108" s="2">
         <v>407.1</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>15</v>
       </c>
@@ -1887,8 +2256,11 @@
       <c r="D109" s="2">
         <v>440.86</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E109" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>15</v>
       </c>
@@ -1901,8 +2273,11 @@
       <c r="D110" s="2">
         <v>236.25</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E110" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>15</v>
       </c>
@@ -1915,8 +2290,11 @@
       <c r="D111" s="2">
         <v>263.11</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E111" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>15</v>
       </c>
@@ -1929,8 +2307,11 @@
       <c r="D112" s="2">
         <v>407.48</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E112" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>15</v>
       </c>
@@ -1943,8 +2324,11 @@
       <c r="D113" s="2">
         <v>399.51</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E113" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>16</v>
       </c>
@@ -1957,8 +2341,11 @@
       <c r="D114" s="2">
         <v>131.96</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E114" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>16</v>
       </c>
@@ -1971,8 +2358,11 @@
       <c r="D115" s="2">
         <v>185.33</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E115" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>16</v>
       </c>
@@ -1985,8 +2375,11 @@
       <c r="D116" s="2">
         <v>209.25</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E116" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>16</v>
       </c>
@@ -1999,8 +2392,11 @@
       <c r="D117" s="2">
         <v>165.92</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E117" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>16</v>
       </c>
@@ -2013,8 +2409,11 @@
       <c r="D118" s="2">
         <v>220.12</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E118" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>16</v>
       </c>
@@ -2027,8 +2426,11 @@
       <c r="D119" s="2">
         <v>169.98</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E119" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>16</v>
       </c>
@@ -2041,8 +2443,11 @@
       <c r="D120" s="2">
         <v>426.59</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E120" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>16</v>
       </c>
@@ -2055,8 +2460,11 @@
       <c r="D121" s="2">
         <v>175.23</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E121" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>16</v>
       </c>
@@ -2069,8 +2477,11 @@
       <c r="D122" s="2">
         <v>284.19</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E122" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>16</v>
       </c>
@@ -2083,8 +2494,11 @@
       <c r="D123" s="2">
         <v>155.72</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E123" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>16</v>
       </c>
@@ -2097,8 +2511,11 @@
       <c r="D124" s="2">
         <v>149.30000000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E124" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>16</v>
       </c>
@@ -2111,8 +2528,11 @@
       <c r="D125" s="2">
         <v>187.67</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E125" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>16</v>
       </c>
@@ -2125,8 +2545,11 @@
       <c r="D126" s="2">
         <v>170.8</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E126" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>16</v>
       </c>
@@ -2139,8 +2562,11 @@
       <c r="D127" s="2">
         <v>300.33999999999997</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E127" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>16</v>
       </c>
@@ -2153,8 +2579,11 @@
       <c r="D128" s="2">
         <v>90.04</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E128" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>16</v>
       </c>
@@ -2167,8 +2596,11 @@
       <c r="D129" s="2">
         <v>280.97000000000003</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E129" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>16</v>
       </c>
@@ -2181,8 +2613,11 @@
       <c r="D130" s="2">
         <v>222.75</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E130" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>16</v>
       </c>
@@ -2195,8 +2630,11 @@
       <c r="D131" s="2">
         <v>229.05</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E131" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>16</v>
       </c>
@@ -2209,8 +2647,11 @@
       <c r="D132" s="2">
         <v>278.64999999999998</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E132" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>16</v>
       </c>
@@ -2223,8 +2664,11 @@
       <c r="D133" s="2">
         <v>160.02000000000001</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E133" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>16</v>
       </c>
@@ -2237,8 +2681,11 @@
       <c r="D134" s="2">
         <v>370.1</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E134" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>16</v>
       </c>
@@ -2251,8 +2698,11 @@
       <c r="D135" s="2">
         <v>198.11</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E135" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>16</v>
       </c>
@@ -2265,8 +2715,11 @@
       <c r="D136" s="2">
         <v>199.76</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E136" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>16</v>
       </c>
@@ -2279,8 +2732,11 @@
       <c r="D137" s="2">
         <v>152.88</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E137" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>16</v>
       </c>
@@ -2293,8 +2749,11 @@
       <c r="D138" s="2">
         <v>189.38</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E138" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>16</v>
       </c>
@@ -2307,8 +2766,11 @@
       <c r="D139" s="2">
         <v>242.06</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E139" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>16</v>
       </c>
@@ -2321,8 +2783,11 @@
       <c r="D140" s="2">
         <v>134.32</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E140" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>16</v>
       </c>
@@ -2335,8 +2800,11 @@
       <c r="D141" s="2">
         <v>336.65</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E141" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>16</v>
       </c>
@@ -2349,8 +2817,11 @@
       <c r="D142" s="2">
         <v>59.62</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E142" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>16</v>
       </c>
@@ -2363,8 +2834,11 @@
       <c r="D143" s="2">
         <v>147.5</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E143" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>16</v>
       </c>
@@ -2377,8 +2851,11 @@
       <c r="D144" s="2">
         <v>112.24</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E144" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>16</v>
       </c>
@@ -2391,8 +2868,11 @@
       <c r="D145" s="2">
         <v>158.74</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E145" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>16</v>
       </c>
@@ -2405,8 +2885,11 @@
       <c r="D146" s="2">
         <v>232.63</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E146" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>16</v>
       </c>
@@ -2419,8 +2902,11 @@
       <c r="D147" s="2">
         <v>289.52</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E147" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>16</v>
       </c>
@@ -2433,8 +2919,11 @@
       <c r="D148" s="2">
         <v>412.75</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E148" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>16</v>
       </c>
@@ -2447,8 +2936,11 @@
       <c r="D149" s="2">
         <v>152.27000000000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E149" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>16</v>
       </c>
@@ -2461,8 +2953,11 @@
       <c r="D150" s="2">
         <v>128.65</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E150" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>16</v>
       </c>
@@ -2475,8 +2970,11 @@
       <c r="D151" s="2">
         <v>169.88</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E151" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>16</v>
       </c>
@@ -2489,8 +2987,11 @@
       <c r="D152" s="2">
         <v>143.22</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E152" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>16</v>
       </c>
@@ -2503,8 +3004,11 @@
       <c r="D153" s="2">
         <v>193.34</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E153" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>16</v>
       </c>
@@ -2517,8 +3021,11 @@
       <c r="D154" s="2">
         <v>208.88</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E154" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>16</v>
       </c>
@@ -2531,8 +3038,11 @@
       <c r="D155" s="2">
         <v>153.94</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E155" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>16</v>
       </c>
@@ -2545,8 +3055,11 @@
       <c r="D156" s="2">
         <v>103.49</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E156" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>16</v>
       </c>
@@ -2559,8 +3072,11 @@
       <c r="D157" s="2">
         <v>240.24</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E157" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>16</v>
       </c>
@@ -2573,8 +3089,11 @@
       <c r="D158" s="2">
         <v>145.57</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E158" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>16</v>
       </c>
@@ -2587,8 +3106,11 @@
       <c r="D159" s="2">
         <v>124.45</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E159" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>16</v>
       </c>
@@ -2601,8 +3123,11 @@
       <c r="D160" s="2">
         <v>190.8</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E160" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>16</v>
       </c>
@@ -2615,8 +3140,11 @@
       <c r="D161" s="2">
         <v>190.06</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E161" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>16</v>
       </c>
@@ -2629,8 +3157,11 @@
       <c r="D162" s="2">
         <v>399.55</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E162" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>16</v>
       </c>
@@ -2643,8 +3174,11 @@
       <c r="D163" s="2">
         <v>189.24</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E163" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>16</v>
       </c>
@@ -2657,8 +3191,11 @@
       <c r="D164" s="2">
         <v>178.3</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E164" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>16</v>
       </c>
@@ -2671,8 +3208,11 @@
       <c r="D165" s="2">
         <v>141.30000000000001</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E165" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>16</v>
       </c>
@@ -2685,8 +3225,11 @@
       <c r="D166" s="2">
         <v>156.30000000000001</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E166" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>16</v>
       </c>
@@ -2699,8 +3242,11 @@
       <c r="D167" s="2">
         <v>167.51</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E167" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>16</v>
       </c>
@@ -2713,8 +3259,11 @@
       <c r="D168" s="2">
         <v>235.17</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E168" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>16</v>
       </c>
@@ -2727,14 +3276,17 @@
       <c r="D169" s="2">
         <v>230.44</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="E169" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3560,6 +4112,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>